<commit_message>
fix the code and enchace
</commit_message>
<xml_diff>
--- a/converted_file.xlsx
+++ b/converted_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliez\Projects\Elisoft-Proj\pvz-preproccesor-product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7826D4E9-A3E7-4E92-A7F0-33C53B0909E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E9CEC96-0D7B-4D36-9704-7200305FDC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="377" yWindow="377" windowWidth="17589" windowHeight="10894" xr2:uid="{677631DF-7FFC-4D53-891F-32A6F83BAE94}"/>
+    <workbookView xWindow="3017" yWindow="3017" windowWidth="17589" windowHeight="10894" xr2:uid="{41DD0664-BBF0-4EEE-B85B-2A6A38B5E211}"/>
   </bookViews>
   <sheets>
     <sheet name="MARCH" sheetId="11" r:id="rId1"/>
@@ -873,9 +873,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{F6B55597-F3B8-4625-A417-E3940579449E}"/>
-    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{DC5F38FC-EF60-4BD1-8523-E57250F76855}"/>
-    <cellStyle name="Normal 2 3" xfId="3" xr:uid="{B3A582E8-2B53-453E-82CE-39B7FB085679}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E55F5653-AC25-4D86-B4BE-B7A3260606EE}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{01D203EF-4574-45C6-BB11-E30FFD986765}"/>
+    <cellStyle name="Normal 2 3" xfId="3" xr:uid="{38227AC1-2CF3-4D07-8E34-4475AE3FD27F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -910,7 +910,7 @@
         <xdr:cNvPr id="368515" name="Picture 1" descr="A close-up of a glass ashtray&#10;&#10;Description automatically generated">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF20F1AF-93CC-C79B-1599-AF768C74967E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7020D0AD-E298-9A3F-FA2E-80BFA151FE12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -984,7 +984,7 @@
         <xdr:cNvPr id="368516" name="Picture 3" descr="A clear glass bowl with measurements&#10;&#10;Description automatically generated">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C76B05C-C91D-7F6E-952D-FDFDCB6415A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C867BF6-80D1-AB22-C6FB-52C80F5B2C0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1058,7 +1058,7 @@
         <xdr:cNvPr id="368517" name="Picture 4" descr="A measuring cup with measurements&#10;&#10;Description automatically generated with medium confidence">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4D17B8E-1827-266F-D29D-5E4B35D6EA63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{100FB439-EAB3-14C3-FAF8-6D9A168589D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1132,7 +1132,7 @@
         <xdr:cNvPr id="368518" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25BA7448-BE8F-2AE7-5B99-DD8FE5EB10C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4463C295-74C7-353F-15A8-01E2C3D2DAE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1206,7 +1206,7 @@
         <xdr:cNvPr id="368519" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D915C0B3-C1A9-E9F2-83E2-92AF948E52BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF31BA18-6D9F-664A-6956-231DDB24C882}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1551,7 +1551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4DC62B4-83C5-4537-97B6-5E0F64CC6FFF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E488A01A-CFB3-4197-8DAE-6F25ABD12F67}">
   <dimension ref="A1:AV11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">

</xml_diff>